<commit_message>
Not sure about this one
</commit_message>
<xml_diff>
--- a/site_DATAexplore/streamPWR.xlsx
+++ b/site_DATAexplore/streamPWR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/site_DATAexplore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7574648A-992A-8941-970C-EC4E7197CC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CADDB1-D08A-E048-AF73-239AD011A98E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>site_id</t>
   </si>
@@ -209,9 +211,6 @@
   </si>
   <si>
     <t>Sstrpwr_2yr</t>
-  </si>
-  <si>
-    <t>ZERO_CowCr</t>
   </si>
   <si>
     <t>ZERO_UmpConf</t>
@@ -248,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1048,13 +1047,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI24"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -1075,7 +1074,7 @@
     <col min="27" max="27" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1152,37 +1151,37 @@
         <v>59</v>
       </c>
       <c r="Z1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" t="s">
         <v>62</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>63</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>64</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>65</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>66</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>67</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH1" t="s">
         <v>68</v>
       </c>
-      <c r="AG1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" t="s">
-        <v>70</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>29.293424643297424</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1325,15 +1324,15 @@
         <v>0.152909674</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E24" si="0" xml:space="preserve"> C3 / 100</f>
+        <f t="shared" ref="E3:E23" si="0" xml:space="preserve"> C3 / 100</f>
         <v>1.41118302E-3</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F24" si="1" xml:space="preserve"> D3 / 100</f>
+        <f t="shared" ref="F3:F23" si="1" xml:space="preserve"> D3 / 100</f>
         <v>1.52909674E-3</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G24" si="2" xml:space="preserve"> (E3 + F3) / 2</f>
+        <f t="shared" ref="G3:G23" si="2" xml:space="preserve"> (E3 + F3) / 2</f>
         <v>1.47013988E-3</v>
       </c>
       <c r="H3">
@@ -1346,7 +1345,7 @@
         <v>160.1308047</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K24" si="3">(H3+I3+J3)/3</f>
+        <f t="shared" ref="K3:K23" si="3">(H3+I3+J3)/3</f>
         <v>187.87781823333333</v>
       </c>
       <c r="L3">
@@ -1368,79 +1367,79 @@
         <v>10600</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R24" si="4">L3*0.02831685</f>
+        <f t="shared" ref="R3:R23" si="4">L3*0.02831685</f>
         <v>1489.46631</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S24" si="5">M3*0.02831685</f>
+        <f t="shared" ref="S3:S23" si="5">M3*0.02831685</f>
         <v>2237.0311500000003</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T24" si="6">N3*0.02831685</f>
+        <f t="shared" ref="T3:T23" si="6">N3*0.02831685</f>
         <v>2749.566135</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U24" si="7">O3 *0.02831685</f>
+        <f t="shared" ref="U3:U23" si="7">O3 *0.02831685</f>
         <v>3398.0219999999999</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V24" si="8">P3 * 0.02831685</f>
+        <f t="shared" ref="V3:V23" si="8">P3 * 0.02831685</f>
         <v>4389.11175</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W24" si="9">Q3 * 0.02831685</f>
+        <f t="shared" ref="W3:W23" si="9">Q3 * 0.02831685</f>
         <v>300.15861000000001</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X24" si="10" xml:space="preserve"> 1000 * 9.8 * R3 * G3</f>
+        <f t="shared" ref="X3:X23" si="10" xml:space="preserve"> 1000 * 9.8 * R3 * G3</f>
         <v>21459.293458024938</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y24" si="11" xml:space="preserve"> X3/K3</f>
+        <f t="shared" ref="Y3:Y23" si="11" xml:space="preserve"> X3/K3</f>
         <v>114.21940950673455</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z24" si="12" xml:space="preserve"> 1000 * 9.8 * S3 * G3</f>
+        <f t="shared" ref="Z3:Z23" si="12" xml:space="preserve"> 1000 * 9.8 * S3 * G3</f>
         <v>32229.737322889174</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA24" si="13" xml:space="preserve"> Z3 / K3</f>
+        <f t="shared" ref="AA3:AA23" si="13" xml:space="preserve"> Z3 / K3</f>
         <v>171.54626142646447</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB24" si="14" xml:space="preserve"> 1000 * 9.8 * T3 * G3</f>
+        <f t="shared" ref="AB3:AB23" si="14" xml:space="preserve"> 1000 * 9.8 * T3 * G3</f>
         <v>39614.018912057443</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC24" si="15" xml:space="preserve"> AB3 / K3</f>
+        <f t="shared" ref="AC3:AC23" si="15" xml:space="preserve"> AB3 / K3</f>
         <v>210.84989853809742</v>
       </c>
       <c r="AD3">
-        <f t="shared" ref="AD3:AD24" si="16" xml:space="preserve"> 1000 * 9.8 * T3 * G3</f>
+        <f t="shared" ref="AD3:AD23" si="16" xml:space="preserve"> 1000 * 9.8 * T3 * G3</f>
         <v>39614.018912057443</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE24" si="17" xml:space="preserve"> AD3/K3</f>
+        <f t="shared" ref="AE3:AE23" si="17" xml:space="preserve"> AD3/K3</f>
         <v>210.84989853809742</v>
       </c>
       <c r="AF3">
-        <f t="shared" ref="AF3:AF24" si="18" xml:space="preserve"> 1000 * 9.8 * V3 * G3</f>
+        <f t="shared" ref="AF3:AF23" si="18" xml:space="preserve"> 1000 * 9.8 * V3 * G3</f>
         <v>63235.560570225578</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG24" si="19" xml:space="preserve"> AF3/K3</f>
+        <f t="shared" ref="AG3:AG23" si="19" xml:space="preserve"> AF3/K3</f>
         <v>336.57810786205044</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH24" si="20" xml:space="preserve"> 1000 * 9.8 * W3 * G3</f>
+        <f t="shared" ref="AH3:AH23" si="20" xml:space="preserve"> 1000 * 9.8 * W3 * G3</f>
         <v>4324.4964002863944</v>
       </c>
       <c r="AI3">
-        <f t="shared" ref="AI3:AI24" si="21" xml:space="preserve"> AH3 / K3</f>
+        <f t="shared" ref="AI3:AI23" si="21" xml:space="preserve"> AH3 / K3</f>
         <v>23.017599634437001</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>13.500120616820508</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1698,7 +1697,7 @@
         <v>35.861137739057099</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>33.834111181041443</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1956,7 +1955,7 @@
         <v>16.454984223522231</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2085,7 +2084,7 @@
         <v>2.3497702146104436</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>35.145533136833116</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>17.161221814971242</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>31.926961914170302</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>5.6204665743334381</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>16.474593099749942</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2859,7 +2858,7 @@
         <v>53.974831678424991</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2988,7 +2987,7 @@
         <v>54.373298572574434</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -3117,7 +3116,7 @@
         <v>76.438441430156502</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>26.452339539723919</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -3375,7 +3374,7 @@
         <v>17.144687172847938</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -3504,7 +3503,7 @@
         <v>35.861137739057099</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>16.454984223522231</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3762,7 +3761,7 @@
         <v>13.500120616820508</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3891,260 +3890,131 @@
         <v>23.017599634437001</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35">
       <c r="A23" t="s">
         <v>60</v>
       </c>
       <c r="B23">
-        <v>2836.1440280000002</v>
+        <v>2473.118743</v>
       </c>
       <c r="C23">
-        <v>0.39666532760444134</v>
+        <v>2.7900075641454664E-2</v>
       </c>
       <c r="D23">
-        <v>0.41641034035666635</v>
+        <v>3.2752086906164671E-2</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>3.9666532760444136E-3</v>
+        <v>2.7900075641454662E-4</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>4.1641034035666633E-3</v>
+        <v>3.2752086906164668E-4</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>4.0653783398055384E-3</v>
+        <v>3.0326081273809662E-4</v>
       </c>
       <c r="H23">
-        <v>61.00517</v>
+        <v>100.33803</v>
       </c>
       <c r="I23">
-        <v>53.14958</v>
+        <v>102.29528999999999</v>
       </c>
       <c r="J23">
-        <v>93.686279999999996</v>
+        <v>164.29221999999999</v>
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
-        <v>69.280343333333334</v>
+        <v>122.30851333333332</v>
       </c>
       <c r="L23">
-        <v>21300</v>
+        <v>62600</v>
       </c>
       <c r="M23">
-        <v>31600</v>
+        <v>94400</v>
       </c>
       <c r="N23">
-        <v>38500</v>
+        <v>116000</v>
       </c>
       <c r="O23">
-        <v>47300</v>
+        <v>144000</v>
       </c>
       <c r="P23">
-        <v>60500</v>
+        <v>186000</v>
       </c>
       <c r="Q23">
-        <v>3110</v>
+        <v>13600</v>
       </c>
       <c r="R23">
         <f t="shared" si="4"/>
-        <v>603.14890500000001</v>
+        <v>1772.63481</v>
       </c>
       <c r="S23">
         <f t="shared" si="5"/>
-        <v>894.81245999999999</v>
+        <v>2673.1106399999999</v>
       </c>
       <c r="T23">
         <f t="shared" si="6"/>
-        <v>1090.198725</v>
+        <v>3284.7546000000002</v>
       </c>
       <c r="U23">
         <f t="shared" si="7"/>
-        <v>1339.387005</v>
+        <v>4077.6264000000001</v>
       </c>
       <c r="V23">
         <f t="shared" si="8"/>
-        <v>1713.169425</v>
+        <v>5266.9341000000004</v>
       </c>
       <c r="W23">
         <f t="shared" si="9"/>
-        <v>88.065403500000002</v>
+        <v>385.10916000000003</v>
       </c>
       <c r="X23">
         <f t="shared" si="10"/>
-        <v>24029.879241831401</v>
+        <v>5268.1925970507264</v>
       </c>
       <c r="Y23">
         <f t="shared" si="11"/>
-        <v>346.8498867884469</v>
+        <v>43.07298366625605</v>
       </c>
       <c r="Z23">
         <f t="shared" si="12"/>
-        <v>35649.96169210667</v>
+        <v>7944.3671112074853</v>
       </c>
       <c r="AA23">
         <f t="shared" si="13"/>
-        <v>514.57541889741412</v>
+        <v>64.953508915248733</v>
       </c>
       <c r="AB23">
         <f t="shared" si="14"/>
-        <v>43434.288770446423</v>
+        <v>9762.1460264837751</v>
       </c>
       <c r="AC23">
         <f t="shared" si="15"/>
-        <v>626.9352413781786</v>
+        <v>79.815752480602271</v>
       </c>
       <c r="AD23">
         <f t="shared" si="16"/>
-        <v>43434.288770446423</v>
+        <v>9762.1460264837751</v>
       </c>
       <c r="AE23">
         <f t="shared" si="17"/>
-        <v>626.9352413781786</v>
+        <v>79.815752480602271</v>
       </c>
       <c r="AF23">
         <f t="shared" si="18"/>
-        <v>68253.882353558671</v>
+        <v>15653.096214879159</v>
       </c>
       <c r="AG23">
         <f t="shared" si="19"/>
-        <v>985.18395073713793</v>
+        <v>127.98043070165538</v>
       </c>
       <c r="AH23">
         <f t="shared" si="20"/>
-        <v>3508.5880019763217</v>
+        <v>1144.5274651739599</v>
       </c>
       <c r="AI23">
-        <f t="shared" si="21"/>
-        <v>50.643340277561968</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24">
-        <v>2473.118743</v>
-      </c>
-      <c r="C24">
-        <v>2.7900075641454664E-2</v>
-      </c>
-      <c r="D24">
-        <v>3.2752086906164671E-2</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>2.7900075641454662E-4</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="1"/>
-        <v>3.2752086906164668E-4</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="2"/>
-        <v>3.0326081273809662E-4</v>
-      </c>
-      <c r="H24">
-        <v>100.33803</v>
-      </c>
-      <c r="I24">
-        <v>102.29528999999999</v>
-      </c>
-      <c r="J24">
-        <v>164.29221999999999</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="3"/>
-        <v>122.30851333333332</v>
-      </c>
-      <c r="L24">
-        <v>62600</v>
-      </c>
-      <c r="M24">
-        <v>94400</v>
-      </c>
-      <c r="N24">
-        <v>116000</v>
-      </c>
-      <c r="O24">
-        <v>144000</v>
-      </c>
-      <c r="P24">
-        <v>186000</v>
-      </c>
-      <c r="Q24">
-        <v>13600</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="4"/>
-        <v>1772.63481</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="5"/>
-        <v>2673.1106399999999</v>
-      </c>
-      <c r="T24">
-        <f t="shared" si="6"/>
-        <v>3284.7546000000002</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="7"/>
-        <v>4077.6264000000001</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="8"/>
-        <v>5266.9341000000004</v>
-      </c>
-      <c r="W24">
-        <f t="shared" si="9"/>
-        <v>385.10916000000003</v>
-      </c>
-      <c r="X24">
-        <f t="shared" si="10"/>
-        <v>5268.1925970507264</v>
-      </c>
-      <c r="Y24">
-        <f t="shared" si="11"/>
-        <v>43.07298366625605</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="12"/>
-        <v>7944.3671112074853</v>
-      </c>
-      <c r="AA24">
-        <f t="shared" si="13"/>
-        <v>64.953508915248733</v>
-      </c>
-      <c r="AB24">
-        <f t="shared" si="14"/>
-        <v>9762.1460264837751</v>
-      </c>
-      <c r="AC24">
-        <f t="shared" si="15"/>
-        <v>79.815752480602271</v>
-      </c>
-      <c r="AD24">
-        <f t="shared" si="16"/>
-        <v>9762.1460264837751</v>
-      </c>
-      <c r="AE24">
-        <f t="shared" si="17"/>
-        <v>79.815752480602271</v>
-      </c>
-      <c r="AF24">
-        <f t="shared" si="18"/>
-        <v>15653.096214879159</v>
-      </c>
-      <c r="AG24">
-        <f t="shared" si="19"/>
-        <v>127.98043070165538</v>
-      </c>
-      <c r="AH24">
-        <f t="shared" si="20"/>
-        <v>1144.5274651739599</v>
-      </c>
-      <c r="AI24">
         <f t="shared" si="21"/>
         <v>9.3577089115188876</v>
       </c>
@@ -4162,12 +4032,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4175,7 +4045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4183,7 +4053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4191,7 +4061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4199,7 +4069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4207,7 +4077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4215,7 +4085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -4223,7 +4093,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -4231,7 +4101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4239,7 +4109,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>56</v>
       </c>

</xml_diff>